<commit_message>
update revised form 2025
</commit_message>
<xml_diff>
--- a/exceljs-pds/PersonalDataSheet.xlsx
+++ b/exceljs-pds/PersonalDataSheet.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66469AC-E3B3-476C-B95E-9BC69B0B0241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880"/>
   </bookViews>
   <sheets>
-    <sheet name="PersonalDataSheet" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="PersonalDataSheet" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="383">
   <si>
     <t>SURNAME</t>
   </si>
@@ -1137,27 +1136,54 @@
   </si>
   <si>
     <t>Govt ID Issue</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, , , </t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>try 11/28/25</t>
+  </si>
+  <si>
+    <t>asdas</t>
+  </si>
+  <si>
+    <t>asdads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1169,7 +1195,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="3" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1542,14 +1568,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:NJ2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:NJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
@@ -1830,7 +1856,7 @@
     <col min="374" max="374" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:374" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="14.4" customHeight="1" spans="1:374" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2954,9 +2980,2256 @@
         <v>373</v>
       </c>
     </row>
-    <row r="2" spans="1:374" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:374" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F2" t="s">
+        <v>375</v>
+      </c>
+      <c r="G2" t="s">
+        <v>376</v>
+      </c>
+      <c r="H2" t="s">
+        <v>377</v>
+      </c>
+      <c r="I2" t="s">
+        <v>375</v>
+      </c>
+      <c r="J2" t="s">
+        <v>375</v>
+      </c>
+      <c r="K2" t="s">
+        <v>375</v>
+      </c>
+      <c r="L2" t="s">
+        <v>375</v>
+      </c>
+      <c r="M2" t="s">
+        <v>375</v>
+      </c>
+      <c r="N2" t="s">
+        <v>375</v>
+      </c>
+      <c r="O2" t="s">
+        <v>375</v>
+      </c>
+      <c r="P2" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>375</v>
+      </c>
+      <c r="R2" t="s">
+        <v>375</v>
+      </c>
+      <c r="S2" t="s">
+        <v>375</v>
+      </c>
+      <c r="T2" t="s">
+        <v>375</v>
+      </c>
+      <c r="U2" t="s">
+        <v>375</v>
+      </c>
+      <c r="V2" t="s">
+        <v>378</v>
+      </c>
+      <c r="W2" t="s">
+        <v>378</v>
+      </c>
+      <c r="X2" t="s">
+        <v>375</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>375</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>374</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>374</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>374</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>374</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>374</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>374</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>375</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>375</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="FZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GN2" t="s">
+        <v>374</v>
+      </c>
+      <c r="GO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GQ2" t="s">
+        <v>374</v>
+      </c>
+      <c r="GR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GS2" t="s">
+        <v>374</v>
+      </c>
+      <c r="GT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GV2" t="s">
+        <v>374</v>
+      </c>
+      <c r="GW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="GZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="ID2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="II2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="IZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="JZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="KZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LL2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="LX2" t="s">
+        <v>379</v>
+      </c>
+      <c r="LY2" t="s">
+        <v>379</v>
+      </c>
+      <c r="LZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MA2" t="s">
+        <v>379</v>
+      </c>
+      <c r="MB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MC2" t="s">
+        <v>379</v>
+      </c>
+      <c r="MD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="ME2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MJ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MK2" t="s">
+        <v>375</v>
+      </c>
+      <c r="ML2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MM2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MN2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MO2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MP2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MQ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MR2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MS2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MT2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MU2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MV2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MW2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MX2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MY2" t="s">
+        <v>375</v>
+      </c>
+      <c r="MZ2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NA2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NB2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NC2" t="s">
+        <v>375</v>
+      </c>
+      <c r="ND2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NE2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NF2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NG2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NH2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NI2" t="s">
+        <v>375</v>
+      </c>
+      <c r="NJ2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:374" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3" t="s">
+        <v>375</v>
+      </c>
+      <c r="E3" t="s">
+        <v>375</v>
+      </c>
+      <c r="F3" t="s">
+        <v>375</v>
+      </c>
+      <c r="G3" t="s">
+        <v>375</v>
+      </c>
+      <c r="H3" t="s">
+        <v>375</v>
+      </c>
+      <c r="I3" t="s">
+        <v>375</v>
+      </c>
+      <c r="J3" t="s">
+        <v>375</v>
+      </c>
+      <c r="K3" t="s">
+        <v>375</v>
+      </c>
+      <c r="L3" t="s">
+        <v>375</v>
+      </c>
+      <c r="M3" t="s">
+        <v>375</v>
+      </c>
+      <c r="N3" t="s">
+        <v>375</v>
+      </c>
+      <c r="O3" t="s">
+        <v>375</v>
+      </c>
+      <c r="P3" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>375</v>
+      </c>
+      <c r="R3" t="s">
+        <v>375</v>
+      </c>
+      <c r="S3" t="s">
+        <v>375</v>
+      </c>
+      <c r="T3" t="s">
+        <v>375</v>
+      </c>
+      <c r="U3" t="s">
+        <v>375</v>
+      </c>
+      <c r="V3" t="s">
+        <v>378</v>
+      </c>
+      <c r="W3" t="s">
+        <v>378</v>
+      </c>
+      <c r="X3" t="s">
+        <v>375</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>375</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="DZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="ED3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="ER3" t="s">
+        <v>375</v>
+      </c>
+      <c r="ES3" t="s">
+        <v>375</v>
+      </c>
+      <c r="ET3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="EZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="FZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="GZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="HZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="ID3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="II3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="IZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="JZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="KZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LL3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="LZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MD3" t="s">
+        <v>375</v>
+      </c>
+      <c r="ME3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MJ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MK3" t="s">
+        <v>375</v>
+      </c>
+      <c r="ML3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MM3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MN3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MO3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MP3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MQ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MR3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MS3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MT3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MU3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MV3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MW3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MX3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MY3" t="s">
+        <v>375</v>
+      </c>
+      <c r="MZ3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NA3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NB3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NC3" t="s">
+        <v>375</v>
+      </c>
+      <c r="ND3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NE3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NF3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NG3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NH3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NI3" t="s">
+        <v>375</v>
+      </c>
+      <c r="NJ3" t="s">
+        <v>375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>